<commit_message>
HACKATHON generateETLInputFiles fully functional (generating data and column mapping files) -added data and column mapping generated example files -updated the mapping doc with data types -real import (very last step) not tested yet
</commit_message>
<xml_diff>
--- a/external/molgenis/TM-Molgenis-mapping.xlsx
+++ b/external/molgenis/TM-Molgenis-mapping.xlsx
@@ -6,13 +6,14 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId3"/>
+    <sheet name="model mapping" sheetId="1" r:id="rId3"/>
+    <sheet name="type mapping" sheetId="2" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>Molgenis</t>
   </si>
@@ -41,9 +42,6 @@
     <t>ObservationSet</t>
   </si>
   <si>
-    <t>ObservationTarget</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -51,6 +49,72 @@
   </si>
   <si>
     <t>ObservationFact (multi-column types)</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>number (0 and 1)</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t>compound</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>number (millis up to day)</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>number (millis up to mills)</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>file (just name)</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>hyperlink</t>
+  </si>
+  <si>
+    <t>image (just name)</t>
+  </si>
+  <si>
+    <t>mref</t>
+  </si>
+  <si>
+    <t>xref</t>
   </si>
 </sst>
 </file>
@@ -83,7 +147,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,6 +163,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -132,7 +202,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -149,6 +219,21 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -170,6 +255,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="fff4f4f4"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -180,7 +266,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozenSplit"/>
@@ -265,7 +351,9 @@
       <c r="B5" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" t="s" s="5">
+        <v>9</v>
+      </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -276,10 +364,10 @@
     <row r="6" ht="20.35" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -290,12 +378,8 @@
     </row>
     <row r="7" ht="20.35" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s" s="5">
-        <v>12</v>
-      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -457,16 +541,265 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
     </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;"Helvetica,Regular"&amp;11&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="0.25" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.5781" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.7266" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="6" customWidth="1"/>
+    <col min="7" max="256" width="12.25" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="2" customHeight="1"/>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="B2" s="2"/>
+      <c r="C2" t="s" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" ht="20.55" customHeight="1">
+      <c r="B3" s="7"/>
+      <c r="C3" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="B4" s="7"/>
+      <c r="C4" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="B5" s="7"/>
+      <c r="C5" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="B6" s="7"/>
+      <c r="C6" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s" s="9">
+        <v>15</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="B7" s="7"/>
+      <c r="C7" t="s" s="5">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="B8" s="7"/>
+      <c r="C8" t="s" s="9">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s" s="9">
+        <v>19</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="B9" s="7"/>
+      <c r="C9" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="B10" s="7"/>
+      <c r="C10" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="B11" s="7"/>
+      <c r="C11" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" ht="20.35" customHeight="1">
+      <c r="B12" s="7"/>
+      <c r="C12" t="s" s="9">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s" s="9">
+        <v>25</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" ht="20.35" customHeight="1">
+      <c r="B13" s="7"/>
+      <c r="C13" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" ht="20.35" customHeight="1">
+      <c r="B14" s="7"/>
+      <c r="C14" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" ht="20.35" customHeight="1">
+      <c r="B15" s="7"/>
+      <c r="C15" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" ht="20.35" customHeight="1">
+      <c r="B16" s="7"/>
+      <c r="C16" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" ht="20.35" customHeight="1">
+      <c r="B17" s="7"/>
+      <c r="C17" t="s" s="5">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" ht="20.35" customHeight="1">
+      <c r="B18" s="7"/>
+      <c r="C18" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" ht="20.35" customHeight="1">
+      <c r="B19" s="7"/>
+      <c r="C19" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" ht="20.35" customHeight="1">
+      <c r="B20" s="7"/>
+      <c r="C20" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" ht="20.35" customHeight="1">
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+    </row>
     <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" ht="20.35" customHeight="1">
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>